<commit_message>
fixed the tree URL
</commit_message>
<xml_diff>
--- a/datasets/Salmonella_enterica_1203NYJAP-1.simulated.xlsx
+++ b/datasets/Salmonella_enterica_1203NYJAP-1.simulated.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="tmpt." localSheetId="0">'Salmonella_enterica_1203NYJAP-1'!$D$10:$D$32</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -441,9 +441,6 @@
     </r>
   </si>
   <si>
-    <t>https://tree.opentreeoflife.org/curator/study/edit/ot_301/tre/tree4.tre</t>
-  </si>
-  <si>
     <t>78f517a041c216ff074f2a96844d5b809dc392899a68b64ab051e6b014cd3c8c</t>
   </si>
   <si>
@@ -583,6 +580,9 @@
   </si>
   <si>
     <t>c3202bf0cfe762d5f345c3f258f07a61607e04f49fc2b0cb94818d105d6ba82f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://api.opentreeoflife.org/v3/study/ot_301/tree/tree4.tre </t>
   </si>
 </sst>
 </file>
@@ -810,9 +810,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="23" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="23" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="23"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1186,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1227,7 @@
         <v>34</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1317,13 +1315,13 @@
         <v>1</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K10" s="18"/>
       <c r="L10" s="18"/>
@@ -1349,10 +1347,10 @@
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
@@ -1378,10 +1376,10 @@
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
@@ -1407,10 +1405,10 @@
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
@@ -1436,10 +1434,10 @@
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
@@ -1465,10 +1463,10 @@
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
@@ -1495,10 +1493,10 @@
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
@@ -1524,10 +1522,10 @@
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
@@ -1553,10 +1551,10 @@
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
@@ -1582,10 +1580,10 @@
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
@@ -1611,10 +1609,10 @@
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
@@ -1640,10 +1638,10 @@
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K21" s="18"/>
       <c r="L21" s="18"/>
@@ -1669,10 +1667,10 @@
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K22" s="18"/>
       <c r="L22" s="18"/>
@@ -1698,10 +1696,10 @@
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K23" s="18"/>
       <c r="L23" s="18"/>
@@ -1727,10 +1725,10 @@
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K24" s="18"/>
       <c r="L24" s="18"/>
@@ -1756,10 +1754,10 @@
       </c>
       <c r="H25" s="16"/>
       <c r="I25" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K25" s="18"/>
       <c r="L25" s="18"/>
@@ -1785,10 +1783,10 @@
       </c>
       <c r="H26" s="16"/>
       <c r="I26" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K26" s="18"/>
       <c r="L26" s="18"/>
@@ -1814,10 +1812,10 @@
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K27" s="18"/>
       <c r="L27" s="18"/>
@@ -1843,10 +1841,10 @@
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K28" s="18"/>
       <c r="L28" s="18"/>
@@ -1872,10 +1870,10 @@
       </c>
       <c r="H29" s="16"/>
       <c r="I29" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
@@ -1901,10 +1899,10 @@
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
@@ -1930,10 +1928,10 @@
       </c>
       <c r="H31" s="16"/>
       <c r="I31" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K31" s="18"/>
       <c r="L31" s="18"/>
@@ -1959,10 +1957,10 @@
       </c>
       <c r="H32" s="16"/>
       <c r="I32" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K32" s="18"/>
       <c r="L32" s="18"/>
@@ -1991,10 +1989,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1" display="https://api.opentreeoflife.org/v3/study/ot_301/tree/tree4.tre"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>